<commit_message>
jay prakash testing jenkins
</commit_message>
<xml_diff>
--- a/public/attach/Project_Plan_Fusion.xlsx
+++ b/public/attach/Project_Plan_Fusion.xlsx
@@ -11,19 +11,20 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$91</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$91</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$F$91</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$F$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$C$1:$C$90</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$91</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$91</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$G$91</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$G$91</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$G$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$G$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$C$1:$C$90</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="124">
   <si>
     <t>#</t>
   </si>
@@ -40,6 +41,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>test status</t>
+  </si>
+  <si>
     <t>Remark</t>
   </si>
   <si>
@@ -58,13 +62,19 @@
     <t>Mayur</t>
   </si>
   <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>No Scroll in document upload in Document system</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
     <t>Completed</t>
   </si>
   <si>
-    <t>No Scroll in document upload in Document system</t>
-  </si>
-  <si>
-    <t>Document</t>
+    <t>done</t>
   </si>
   <si>
     <t>No Scroll in Bug creation</t>
@@ -73,6 +83,9 @@
     <t>Bug</t>
   </si>
   <si>
+    <t>not done</t>
+  </si>
+  <si>
     <t>Add filter on top of each column in view bug screen</t>
   </si>
   <si>
@@ -86,6 +99,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>not done for view bug page, project resources, asset assign, timesheet.</t>
   </si>
   <si>
     <t>Asset Admin access to be given to some person</t>
@@ -140,6 +156,9 @@
     <t>Notifications for all Modules</t>
   </si>
   <si>
+    <t>only on bug, timesheet</t>
+  </si>
+  <si>
     <t>Resource View to have resource total effort by project and all project together</t>
   </si>
   <si>
@@ -212,9 +231,6 @@
     <t>Super Admin, login control i.e super Admin can see which companies are registered with registered user login details. Super Admin can stop a company to login and all users in that company will be prohibited to login</t>
   </si>
   <si>
-    <t>WIP</t>
-  </si>
-  <si>
     <t>Excel download and uploads</t>
   </si>
   <si>
@@ -269,6 +285,9 @@
     <t>Add filter to all values in Project plan</t>
   </si>
   <si>
+    <t>not according to requirement</t>
+  </si>
+  <si>
     <t>Provide access to a plan ( display) to any resource</t>
   </si>
   <si>
@@ -311,6 +330,9 @@
     <t>A Icon at the top to export the plan in excel</t>
   </si>
   <si>
+    <t>breaks the application</t>
+  </si>
+  <si>
     <t>A Icon at the top to print the plan</t>
   </si>
   <si>
@@ -357,6 +379,9 @@
   </si>
   <si>
     <t>Load a file and then immediately click on other module, File does not load</t>
+  </si>
+  <si>
+    <t>Not done</t>
   </si>
   <si>
     <t>in History, for a round latest status should be shown in Interview schedule history section</t>
@@ -491,13 +516,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -506,12 +531,13 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.4387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8163265306122"/>
     <col collapsed="false" hidden="true" max="4" min="4" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="212.214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="212.214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,8 +553,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -536,78 +565,89 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -615,184 +655,214 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,29 +870,33 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,59 +904,65 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,221 +970,249 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="n">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="n">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,309 +1220,333 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="n">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="n">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="n">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="n">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="n">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="n">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="n">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="n">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="n">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="n">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="n">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="n">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="n">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="n">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="n">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F55" s="1"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="n">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="n">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="n">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,140 +1554,163 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="n">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="n">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="n">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="n">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="n">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="n">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="n">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="n">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,33 +1718,37 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="n">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,31 +1756,35 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="n">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1629,80 +1792,89 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="n">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="n">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="n">
         <v>75</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="n">
         <v>76</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,246 +1882,258 @@
         <v>77</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="n">
         <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="n">
         <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F79" s="1"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="n">
         <v>80</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F80" s="1"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="n">
         <v>81</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="n">
         <v>82</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="n">
         <v>83</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="F83" s="1"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="n">
         <v>84</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="F84" s="1"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="n">
         <v>85</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="n">
         <v>86</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="n">
         <v>87</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F87" s="1"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="n">
         <v>88</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F88" s="1"/>
     </row>
     <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="n">
         <v>89</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F89" s="1"/>
     </row>
     <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="n">
         <v>90</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F90" s="1"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>91</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F91" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F91">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="WIP"/>
-        <filter val="Rejected"/>
-        <filter val="Partialy completed"/>
-        <filter val="Not Started"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G91"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>